<commit_message>
Farklı packageler oluşturarak classlarımı düzenledim, tabloya databaseden veri çektim ve excel export buttonumu aktifleştirdim.
</commit_message>
<xml_diff>
--- a/newProjekt/MagneticReport.xlsx
+++ b/newProjekt/MagneticReport.xlsx
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -2615,6 +2615,18 @@
   </si>
   <si>
     <t>Doküman No: F.02 Yayın Tarihi : 01.05.2018 Revizyon No :01 Revizyon Tarihi :19.03.2019</t>
+  </si>
+  <si>
+    <t>SARI GEMİ</t>
+  </si>
+  <si>
+    <t>ARSLAN PROJE</t>
+  </si>
+  <si>
+    <t>İSTANBUL</t>
+  </si>
+  <si>
+    <t>ARSLAN GEMİ</t>
   </si>
 </sst>
 </file>
@@ -2622,14 +2634,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="#."/>
     <numFmt numFmtId="178" formatCode="#.00"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="m\o\n\th\ d\,\ yyyy"/>
     <numFmt numFmtId="181" formatCode="General_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="45">
     <font>
@@ -3813,7 +3825,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4230,6 +4242,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -4795,32 +4816,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81904761904762" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.26666666666667" style="3" customWidth="1"/>
-    <col min="2" max="3" width="5.26666666666667" style="3" customWidth="1"/>
-    <col min="4" max="4" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4.72380952380952" style="3" customWidth="1"/>
-    <col min="6" max="6" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="7" max="7" width="4.18095238095238" style="3" customWidth="1"/>
-    <col min="8" max="8" width="3.26666666666667" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.54285714285714" style="3" customWidth="1"/>
-    <col min="10" max="10" width="3.45714285714286" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.72380952380952" style="3" customWidth="1"/>
-    <col min="12" max="12" width="4.81904761904762" style="3" customWidth="1"/>
-    <col min="13" max="15" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.72380952380952" style="3" customWidth="1"/>
-    <col min="17" max="17" width="3.72380952380952" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.7238095238095" style="3" customWidth="1"/>
-    <col min="19" max="19" width="4.81904761904762" style="3" customWidth="1"/>
-    <col min="20" max="20" width="3.81904761904762" style="3" customWidth="1"/>
-    <col min="21" max="21" width="3.45714285714286" style="3" customWidth="1"/>
-    <col min="22" max="22" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.7238095238095" style="3" customWidth="1"/>
-    <col min="24" max="24" width="2.45714285714286" style="3" customWidth="1"/>
-    <col min="25" max="25" width="5.72380952380952" style="3" customWidth="1"/>
-    <col min="26" max="26" width="4.72380952380952" style="3" customWidth="1"/>
-    <col min="27" max="27" width="6.72380952380952" style="3" customWidth="1"/>
-    <col min="28" max="28" width="7.81904761904762" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="8.81904761904762" style="3"/>
+    <col min="1" max="1" customWidth="true" style="3" width="7.26666666666667" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="3" width="5.26666666666667" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="4.18095238095238" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="3.26666666666667" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="5.54285714285714" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
+    <col min="13" max="15" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="3" width="8.72380952380952" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="3" width="3.72380952380952" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="3" width="3.81904761904762" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="2.45714285714286" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="6.72380952380952" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="7.81904761904762" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="8.81904761904762" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="31.9" customHeight="1" spans="1:28">
@@ -4893,7 +4914,9 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
+      <c r="D3" t="s" s="143">
+        <v>85</v>
+      </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -4929,7 +4952,9 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="D4" t="s" s="143">
+        <v>83</v>
+      </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
@@ -4965,7 +4990,9 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="19"/>
+      <c r="D5" t="s" s="143">
+        <v>84</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -7004,10 +7031,10 @@
   <headerFooter/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x14">
       <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:AlternateContent>
           <mc:Choice Requires="x14">
             <control shapeId="11268" name="Check Box 4" r:id="rId4">
               <controlPr defaultSize="0">
@@ -7029,7 +7056,7 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:AlternateContent>
           <mc:Choice Requires="x14">
             <control shapeId="11269" name="Check Box 5" r:id="rId5">
               <controlPr defaultSize="0">

</xml_diff>

<commit_message>
raportOlusturma sayfasının gui designını yaptım, rapor için comboboxlara veri çektim ve rapora gönderdim ve excele aktardım.
</commit_message>
<xml_diff>
--- a/newProjekt/MagneticReport.xlsx
+++ b/newProjekt/MagneticReport.xlsx
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -1347,6 +1347,9 @@
     </r>
   </si>
   <si>
+    <t>SARI GEMİ</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1410,6 +1413,9 @@
     </r>
   </si>
   <si>
+    <t>ARSLAN PROJE</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1471,6 +1477,9 @@
       </rPr>
       <t xml:space="preserve">Inspection Place </t>
     </r>
+  </si>
+  <si>
+    <t>İSTANBUL</t>
   </si>
   <si>
     <r>
@@ -2531,13 +2540,13 @@
     </r>
   </si>
   <si>
-    <t>fsdf</t>
-  </si>
-  <si>
-    <t>fadsfsadf</t>
-  </si>
-  <si>
-    <t>fasdfdsaf</t>
+    <t>ali alkan</t>
+  </si>
+  <si>
+    <t>burcu yıldız</t>
+  </si>
+  <si>
+    <t>şevval arslan</t>
   </si>
   <si>
     <r>
@@ -2560,12 +2569,6 @@
     </r>
   </si>
   <si>
-    <t>LEVEL 2</t>
-  </si>
-  <si>
-    <t>LEVEL 3</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2615,18 +2618,6 @@
   </si>
   <si>
     <t>Doküman No: F.02 Yayın Tarihi : 01.05.2018 Revizyon No :01 Revizyon Tarihi :19.03.2019</t>
-  </si>
-  <si>
-    <t>SARI GEMİ</t>
-  </si>
-  <si>
-    <t>ARSLAN PROJE</t>
-  </si>
-  <si>
-    <t>İSTANBUL</t>
-  </si>
-  <si>
-    <t>ARSLAN GEMİ</t>
   </si>
 </sst>
 </file>
@@ -2636,14 +2627,14 @@
   <numFmts count="8">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="#."/>
-    <numFmt numFmtId="178" formatCode="#.00"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="m\o\n\th\ d\,\ yyyy"/>
-    <numFmt numFmtId="181" formatCode="General_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="#.00"/>
+    <numFmt numFmtId="178" formatCode="m\o\n\th\ d\,\ yyyy"/>
+    <numFmt numFmtId="179" formatCode="General_)"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="#."/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="44">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2672,14 +2663,6 @@
       <u/>
       <sz val="9"/>
       <color theme="5" tint="-0.25"/>
-      <name val="Arial"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <charset val="162"/>
     </font>
@@ -2729,6 +2712,14 @@
       <charset val="162"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2736,11 +2727,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="1"/>
-      <color indexed="8"/>
-      <name val="Courier"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2751,21 +2750,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="1"/>
-      <color indexed="8"/>
-      <name val="Courier"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <charset val="162"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2783,43 +2771,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2841,39 +2800,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <sz val="1"/>
+      <color indexed="8"/>
+      <name val="Courier"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2887,12 +2853,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="1"/>
+      <color indexed="8"/>
+      <name val="Courier"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <charset val="162"/>
     </font>
     <font>
       <b/>
@@ -2957,25 +2940,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2987,7 +2958,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3011,7 +3018,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3023,13 +3030,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3047,13 +3048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3065,19 +3066,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3089,55 +3120,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3566,11 +3549,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3597,21 +3619,6 @@
       </top>
       <bottom style="double">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3639,42 +3646,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3684,148 +3667,148 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="18" fillId="0" borderId="0">
+    <xf numFmtId="178" fontId="27" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="27" fillId="0" borderId="39">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="27" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="36">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="18" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="181" fontId="33" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="181" fontId="33" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3864,6 +3847,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3876,25 +3862,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3918,7 +3898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3927,88 +3907,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4017,25 +3997,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4047,20 +4027,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4096,13 +4073,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4111,16 +4088,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4150,34 +4127,37 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4210,31 +4190,31 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4242,15 +4222,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -4810,38 +4781,38 @@
   <sheetPr/>
   <dimension ref="A1:AB429"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:P3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Z40" sqref="Z40:AB40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81904761904762" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="7.26666666666667" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="3" width="5.26666666666667" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="4.18095238095238" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="3.26666666666667" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="5.54285714285714" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
-    <col min="13" max="15" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="3" width="8.72380952380952" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="3" width="3.72380952380952" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="3" width="3.81904761904762" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="3" width="2.45714285714286" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="3" width="6.72380952380952" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="3" width="7.81904761904762" collapsed="true"/>
-    <col min="29" max="16384" style="3" width="8.81904761904762" collapsed="true"/>
+    <col min="1" max="1" width="7.26666666666667" style="3" customWidth="1"/>
+    <col min="2" max="3" width="5.26666666666667" style="3" customWidth="1"/>
+    <col min="4" max="4" width="0.819047619047619" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4.72380952380952" style="3" customWidth="1"/>
+    <col min="6" max="6" width="0.819047619047619" style="3" customWidth="1"/>
+    <col min="7" max="7" width="4.18095238095238" style="3" customWidth="1"/>
+    <col min="8" max="8" width="3.26666666666667" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.54285714285714" style="3" customWidth="1"/>
+    <col min="10" max="10" width="3.45714285714286" style="3" customWidth="1"/>
+    <col min="11" max="11" width="5.72380952380952" style="3" customWidth="1"/>
+    <col min="12" max="12" width="4.81904761904762" style="3" customWidth="1"/>
+    <col min="13" max="15" width="0.819047619047619" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.72380952380952" style="3" customWidth="1"/>
+    <col min="17" max="17" width="3.72380952380952" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.7238095238095" style="3" customWidth="1"/>
+    <col min="19" max="19" width="4.81904761904762" style="3" customWidth="1"/>
+    <col min="20" max="20" width="3.81904761904762" style="3" customWidth="1"/>
+    <col min="21" max="21" width="3.45714285714286" style="3" customWidth="1"/>
+    <col min="22" max="22" width="0.819047619047619" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.7238095238095" style="3" customWidth="1"/>
+    <col min="24" max="24" width="2.45714285714286" style="3" customWidth="1"/>
+    <col min="25" max="25" width="5.72380952380952" style="3" customWidth="1"/>
+    <col min="26" max="26" width="4.72380952380952" style="3" customWidth="1"/>
+    <col min="27" max="27" width="6.72380952380952" style="3" customWidth="1"/>
+    <col min="28" max="28" width="7.81904761904762" style="3" customWidth="1"/>
+    <col min="29" max="16384" width="8.81904761904762" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="31.9" customHeight="1" spans="1:28">
@@ -4855,26 +4826,26 @@
       <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="110"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="108"/>
     </row>
     <row r="2" ht="43.15" customHeight="1" spans="1:28">
       <c r="A2" s="8"/>
@@ -4887,26 +4858,26 @@
       <c r="H2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="68"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="111"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="109"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="28.15" customHeight="1" spans="1:28">
       <c r="A3" s="12" t="s">
@@ -4914,46 +4885,46 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" t="s" s="143">
-        <v>85</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="77" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="75" t="s">
+        <v>4</v>
       </c>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="77" t="s">
-        <v>4</v>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="75" t="s">
+        <v>5</v>
       </c>
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="113"/>
+      <c r="AA3" s="110"/>
+      <c r="AB3" s="111"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="28.15" customHeight="1" spans="1:28">
-      <c r="A4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" t="s" s="143">
-        <v>83</v>
+      <c r="A4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -4967,31 +4938,31 @@
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
-      <c r="Q4" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="114"/>
+      <c r="Q4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="113"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="28.15" customHeight="1" spans="1:28">
-      <c r="A5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" t="s" s="143">
-        <v>84</v>
+      <c r="A5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
@@ -5005,29 +4976,29 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
-      <c r="Q5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="114"/>
+      <c r="Q5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="114"/>
+      <c r="AB5" s="113"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="28.15" customHeight="1" spans="1:28">
-      <c r="A6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
@@ -5041,1402 +5012,1390 @@
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
-      <c r="Q6" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="114"/>
+      <c r="Q6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="112"/>
+      <c r="AB6" s="113"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="28.15" customHeight="1" spans="1:28">
-      <c r="A7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="82"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="82"/>
-      <c r="W7" s="82"/>
-      <c r="X7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="116"/>
+      <c r="A7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="115"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="18.65" customHeight="1" spans="1:28">
-      <c r="A8" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="117"/>
+      <c r="A8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="116"/>
     </row>
     <row r="9" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="118"/>
+      <c r="A9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="117"/>
     </row>
     <row r="10" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="72"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="118"/>
+      <c r="A10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="117"/>
     </row>
     <row r="11" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="72"/>
-      <c r="Y11" s="72"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="118"/>
+      <c r="A11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="71"/>
+      <c r="Y11" s="71"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="117"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="119"/>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="120"/>
+      <c r="A12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="118"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="119"/>
     </row>
     <row r="13" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="83" t="s">
-        <v>31</v>
-      </c>
-      <c r="X13" s="84"/>
-      <c r="Y13" s="121"/>
-      <c r="Z13" s="122"/>
-      <c r="AA13" s="123"/>
-      <c r="AB13" s="124"/>
+      <c r="A13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="X13" s="82"/>
+      <c r="Y13" s="120"/>
+      <c r="Z13" s="121"/>
+      <c r="AA13" s="122"/>
+      <c r="AB13" s="123"/>
     </row>
     <row r="14" ht="27.65" customHeight="1" spans="1:28">
-      <c r="A14" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="86" t="s">
-        <v>34</v>
-      </c>
-      <c r="X14" s="87"/>
-      <c r="Y14" s="125"/>
-      <c r="Z14" s="126"/>
-      <c r="AA14" s="127"/>
-      <c r="AB14" s="128"/>
+      <c r="A14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="83"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="X14" s="85"/>
+      <c r="Y14" s="124"/>
+      <c r="Z14" s="125"/>
+      <c r="AA14" s="126"/>
+      <c r="AB14" s="127"/>
     </row>
     <row r="15" ht="19.9" customHeight="1" spans="1:28">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="88" t="s">
-        <v>35</v>
-      </c>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
-      <c r="W15" s="89"/>
-      <c r="X15" s="89"/>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="89"/>
-      <c r="AA15" s="89"/>
-      <c r="AB15" s="129"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="87"/>
+      <c r="S15" s="87"/>
+      <c r="T15" s="87"/>
+      <c r="U15" s="87"/>
+      <c r="V15" s="87"/>
+      <c r="W15" s="87"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
+      <c r="Z15" s="87"/>
+      <c r="AA15" s="87"/>
+      <c r="AB15" s="128"/>
     </row>
     <row r="16" ht="19.9" customHeight="1" spans="1:28">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="R16" s="91"/>
-      <c r="S16" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="T16" s="92"/>
-      <c r="U16" s="92"/>
-      <c r="V16" s="92"/>
-      <c r="W16" s="92"/>
-      <c r="X16" s="92"/>
-      <c r="Y16" s="92"/>
-      <c r="Z16" s="92"/>
-      <c r="AA16" s="92"/>
-      <c r="AB16" s="130"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="R16" s="89"/>
+      <c r="S16" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16" s="90"/>
+      <c r="U16" s="90"/>
+      <c r="V16" s="90"/>
+      <c r="W16" s="90"/>
+      <c r="X16" s="90"/>
+      <c r="Y16" s="90"/>
+      <c r="Z16" s="90"/>
+      <c r="AA16" s="90"/>
+      <c r="AB16" s="129"/>
     </row>
     <row r="17" ht="19.9" customHeight="1" spans="1:28">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="93" t="s">
-        <v>38</v>
-      </c>
-      <c r="R17" s="91"/>
-      <c r="S17" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="T17" s="92"/>
-      <c r="U17" s="92"/>
-      <c r="V17" s="92"/>
-      <c r="W17" s="92"/>
-      <c r="X17" s="92"/>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="92"/>
-      <c r="AA17" s="92"/>
-      <c r="AB17" s="130"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" s="89"/>
+      <c r="S17" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="T17" s="90"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="90"/>
+      <c r="AA17" s="90"/>
+      <c r="AB17" s="129"/>
     </row>
     <row r="18" ht="19.9" customHeight="1" spans="1:28">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="93" t="s">
-        <v>40</v>
-      </c>
-      <c r="R18" s="91"/>
-      <c r="S18" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="T18" s="92"/>
-      <c r="U18" s="92"/>
-      <c r="V18" s="92"/>
-      <c r="W18" s="92"/>
-      <c r="X18" s="92"/>
-      <c r="Y18" s="92"/>
-      <c r="Z18" s="92"/>
-      <c r="AA18" s="92"/>
-      <c r="AB18" s="130"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="89"/>
+      <c r="S18" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="129"/>
     </row>
     <row r="19" ht="19.9" customHeight="1" spans="1:28">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="95" t="s">
-        <v>42</v>
-      </c>
-      <c r="R19" s="96"/>
-      <c r="S19" s="97" t="s">
-        <v>43</v>
-      </c>
-      <c r="T19" s="97"/>
-      <c r="U19" s="97"/>
-      <c r="V19" s="97"/>
-      <c r="W19" s="97"/>
-      <c r="X19" s="97"/>
-      <c r="Y19" s="97"/>
-      <c r="Z19" s="97"/>
-      <c r="AA19" s="97"/>
-      <c r="AB19" s="131"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="R19" s="94"/>
+      <c r="S19" s="95" t="s">
+        <v>46</v>
+      </c>
+      <c r="T19" s="95"/>
+      <c r="U19" s="95"/>
+      <c r="V19" s="95"/>
+      <c r="W19" s="95"/>
+      <c r="X19" s="95"/>
+      <c r="Y19" s="95"/>
+      <c r="Z19" s="95"/>
+      <c r="AA19" s="95"/>
+      <c r="AB19" s="130"/>
     </row>
     <row r="20" ht="26.5" customHeight="1" spans="1:28">
-      <c r="A20" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="98"/>
-      <c r="R20" s="98"/>
-      <c r="S20" s="98"/>
-      <c r="T20" s="98"/>
-      <c r="U20" s="98"/>
-      <c r="V20" s="98"/>
-      <c r="W20" s="98"/>
-      <c r="X20" s="98"/>
-      <c r="Y20" s="98"/>
-      <c r="Z20" s="98"/>
-      <c r="AA20" s="98"/>
-      <c r="AB20" s="132"/>
+      <c r="A20" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="96"/>
+      <c r="R20" s="96"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="96"/>
+      <c r="U20" s="96"/>
+      <c r="V20" s="96"/>
+      <c r="W20" s="96"/>
+      <c r="X20" s="96"/>
+      <c r="Y20" s="96"/>
+      <c r="Z20" s="96"/>
+      <c r="AA20" s="96"/>
+      <c r="AB20" s="131"/>
     </row>
     <row r="21" ht="26.5" customHeight="1" spans="1:28">
-      <c r="A21" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="71"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="71"/>
-      <c r="Y21" s="71"/>
-      <c r="Z21" s="71"/>
-      <c r="AA21" s="71"/>
-      <c r="AB21" s="133"/>
+      <c r="A21" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="70"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="70"/>
+      <c r="V21" s="70"/>
+      <c r="W21" s="70"/>
+      <c r="X21" s="70"/>
+      <c r="Y21" s="70"/>
+      <c r="Z21" s="70"/>
+      <c r="AA21" s="70"/>
+      <c r="AB21" s="132"/>
     </row>
     <row r="22" ht="26.5" customHeight="1" spans="1:28">
-      <c r="A22" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="44"/>
-      <c r="Z22" s="44"/>
-      <c r="AA22" s="44"/>
-      <c r="AB22" s="134"/>
+      <c r="A22" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="133"/>
     </row>
     <row r="23" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A23" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="46"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="46"/>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="46"/>
-      <c r="AB23" s="135"/>
+      <c r="A23" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="134"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="28.9" customHeight="1" spans="1:28">
-      <c r="A24" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="72" t="s">
+      <c r="A24" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="48" t="s">
+      <c r="B24" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="S24" s="48" t="s">
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="99" t="s">
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="X24" s="100"/>
-      <c r="Y24" s="48" t="s">
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="Z24" s="49"/>
-      <c r="AA24" s="49"/>
-      <c r="AB24" s="136" t="s">
+      <c r="S24" s="47" t="s">
         <v>56</v>
+      </c>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
+      <c r="W24" s="97" t="s">
+        <v>57</v>
+      </c>
+      <c r="X24" s="98"/>
+      <c r="Y24" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="135" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A25" s="50">
+      <c r="A25" s="49">
         <v>1</v>
       </c>
-      <c r="B25" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="73">
+      <c r="B25" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="72">
         <v>300</v>
       </c>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="73">
+      <c r="J25" s="72"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="72"/>
+      <c r="Q25" s="72"/>
+      <c r="R25" s="72">
         <v>12</v>
       </c>
-      <c r="S25" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T25" s="101"/>
-      <c r="U25" s="101"/>
-      <c r="V25" s="101"/>
-      <c r="W25" s="102"/>
-      <c r="X25" s="103"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="34"/>
-      <c r="AB25" s="137" t="s">
-        <v>60</v>
+      <c r="S25" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="T25" s="99"/>
+      <c r="U25" s="99"/>
+      <c r="V25" s="99"/>
+      <c r="W25" s="100"/>
+      <c r="X25" s="101"/>
+      <c r="Y25" s="33"/>
+      <c r="Z25" s="33"/>
+      <c r="AA25" s="33"/>
+      <c r="AB25" s="136" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A26" s="50">
+      <c r="A26" s="49">
         <v>2</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="72">
+        <v>300</v>
+      </c>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="73">
-        <v>300</v>
-      </c>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
-      <c r="P26" s="73"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="73">
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="72"/>
+      <c r="Q26" s="72"/>
+      <c r="R26" s="72">
         <v>12</v>
       </c>
-      <c r="S26" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T26" s="101"/>
-      <c r="U26" s="101"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="102"/>
-      <c r="X26" s="103"/>
-      <c r="Y26" s="34"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="34"/>
-      <c r="AB26" s="137" t="s">
-        <v>60</v>
+      <c r="S26" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="T26" s="99"/>
+      <c r="U26" s="99"/>
+      <c r="V26" s="99"/>
+      <c r="W26" s="100"/>
+      <c r="X26" s="101"/>
+      <c r="Y26" s="33"/>
+      <c r="Z26" s="33"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="136" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A27" s="50">
+      <c r="A27" s="49">
         <v>3</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="72">
+        <v>300</v>
+      </c>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72">
+        <v>12</v>
+      </c>
+      <c r="S27" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="73">
-        <v>300</v>
-      </c>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="73"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="73">
-        <v>12</v>
-      </c>
-      <c r="S27" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T27" s="101"/>
-      <c r="U27" s="101"/>
-      <c r="V27" s="101"/>
-      <c r="W27" s="102"/>
-      <c r="X27" s="103"/>
-      <c r="Y27" s="34"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="34"/>
-      <c r="AB27" s="137" t="s">
-        <v>60</v>
+      <c r="T27" s="99"/>
+      <c r="U27" s="99"/>
+      <c r="V27" s="99"/>
+      <c r="W27" s="100"/>
+      <c r="X27" s="101"/>
+      <c r="Y27" s="33"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="136" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A28" s="50">
+      <c r="A28" s="49">
         <v>4</v>
       </c>
-      <c r="B28" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="73">
+      <c r="B28" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="72">
         <v>300</v>
       </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73" t="s">
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="72"/>
+      <c r="R28" s="72">
+        <v>12</v>
+      </c>
+      <c r="S28" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="T28" s="99"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="99"/>
+      <c r="W28" s="100"/>
+      <c r="X28" s="101"/>
+      <c r="Y28" s="33"/>
+      <c r="Z28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="136" t="s">
         <v>63</v>
-      </c>
-      <c r="M28" s="73"/>
-      <c r="N28" s="73"/>
-      <c r="O28" s="73"/>
-      <c r="P28" s="73"/>
-      <c r="Q28" s="73"/>
-      <c r="R28" s="73">
-        <v>12</v>
-      </c>
-      <c r="S28" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T28" s="101"/>
-      <c r="U28" s="101"/>
-      <c r="V28" s="101"/>
-      <c r="W28" s="102"/>
-      <c r="X28" s="103"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="34"/>
-      <c r="AB28" s="137" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A29" s="50">
+      <c r="A29" s="49">
         <v>5</v>
       </c>
-      <c r="B29" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="73">
+      <c r="B29" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="72">
         <v>300</v>
       </c>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73" t="s">
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="72"/>
+      <c r="R29" s="72">
+        <v>12</v>
+      </c>
+      <c r="S29" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="T29" s="99"/>
+      <c r="U29" s="99"/>
+      <c r="V29" s="99"/>
+      <c r="W29" s="100"/>
+      <c r="X29" s="101"/>
+      <c r="Y29" s="33"/>
+      <c r="Z29" s="33"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="136" t="s">
         <v>63</v>
-      </c>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="73">
-        <v>12</v>
-      </c>
-      <c r="S29" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T29" s="101"/>
-      <c r="U29" s="101"/>
-      <c r="V29" s="101"/>
-      <c r="W29" s="102"/>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="34"/>
-      <c r="Z29" s="34"/>
-      <c r="AA29" s="34"/>
-      <c r="AB29" s="137" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A30" s="50">
+      <c r="A30" s="49">
         <v>6</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="72">
+        <v>300</v>
+      </c>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
+      <c r="O30" s="72"/>
+      <c r="P30" s="72"/>
+      <c r="Q30" s="72"/>
+      <c r="R30" s="72">
+        <v>12</v>
+      </c>
+      <c r="S30" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="73">
-        <v>300</v>
-      </c>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73" t="s">
+      <c r="T30" s="99"/>
+      <c r="U30" s="99"/>
+      <c r="V30" s="99"/>
+      <c r="W30" s="100"/>
+      <c r="X30" s="101"/>
+      <c r="Y30" s="33"/>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="136" t="s">
         <v>63</v>
-      </c>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
-      <c r="O30" s="73"/>
-      <c r="P30" s="73"/>
-      <c r="Q30" s="73"/>
-      <c r="R30" s="73">
-        <v>12</v>
-      </c>
-      <c r="S30" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="T30" s="101"/>
-      <c r="U30" s="101"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="102"/>
-      <c r="X30" s="103"/>
-      <c r="Y30" s="34"/>
-      <c r="Z30" s="34"/>
-      <c r="AA30" s="34"/>
-      <c r="AB30" s="137" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="31" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A31" s="50">
+      <c r="A31" s="49">
         <v>7</v>
       </c>
-      <c r="B31" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="73">
+      <c r="B31" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="72">
         <v>300</v>
       </c>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="73"/>
-      <c r="Q31" s="73"/>
-      <c r="R31" s="73">
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
+      <c r="Q31" s="72"/>
+      <c r="R31" s="72">
         <v>4</v>
       </c>
-      <c r="S31" s="101" t="s">
-        <v>66</v>
-      </c>
-      <c r="T31" s="101"/>
-      <c r="U31" s="101"/>
-      <c r="V31" s="101"/>
-      <c r="W31" s="102"/>
-      <c r="X31" s="103"/>
-      <c r="Y31" s="34"/>
-      <c r="Z31" s="34"/>
-      <c r="AA31" s="34"/>
-      <c r="AB31" s="137" t="s">
-        <v>60</v>
+      <c r="S31" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="T31" s="99"/>
+      <c r="U31" s="99"/>
+      <c r="V31" s="99"/>
+      <c r="W31" s="100"/>
+      <c r="X31" s="101"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="33"/>
+      <c r="AA31" s="33"/>
+      <c r="AB31" s="136" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A32" s="50">
+      <c r="A32" s="49">
         <v>8</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="73"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="73"/>
-      <c r="Q32" s="73"/>
-      <c r="R32" s="73"/>
-      <c r="S32" s="101"/>
-      <c r="T32" s="101"/>
-      <c r="U32" s="101"/>
-      <c r="V32" s="101"/>
-      <c r="W32" s="102"/>
-      <c r="X32" s="103"/>
-      <c r="Y32" s="34"/>
-      <c r="Z32" s="34"/>
-      <c r="AA32" s="34"/>
-      <c r="AB32" s="137"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="72"/>
+      <c r="O32" s="72"/>
+      <c r="P32" s="72"/>
+      <c r="Q32" s="72"/>
+      <c r="R32" s="72"/>
+      <c r="S32" s="99"/>
+      <c r="T32" s="99"/>
+      <c r="U32" s="99"/>
+      <c r="V32" s="99"/>
+      <c r="W32" s="100"/>
+      <c r="X32" s="101"/>
+      <c r="Y32" s="33"/>
+      <c r="Z32" s="33"/>
+      <c r="AA32" s="33"/>
+      <c r="AB32" s="136"/>
     </row>
     <row r="33" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A33" s="50">
+      <c r="A33" s="49">
         <v>9</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="73"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="73"/>
-      <c r="S33" s="101"/>
-      <c r="T33" s="101"/>
-      <c r="U33" s="101"/>
-      <c r="V33" s="101"/>
-      <c r="W33" s="102"/>
-      <c r="X33" s="103"/>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="34"/>
-      <c r="AB33" s="137"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="99"/>
+      <c r="T33" s="99"/>
+      <c r="U33" s="99"/>
+      <c r="V33" s="99"/>
+      <c r="W33" s="100"/>
+      <c r="X33" s="101"/>
+      <c r="Y33" s="33"/>
+      <c r="Z33" s="33"/>
+      <c r="AA33" s="33"/>
+      <c r="AB33" s="136"/>
     </row>
     <row r="34" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A34" s="50">
+      <c r="A34" s="49">
         <v>10</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="73"/>
-      <c r="S34" s="101"/>
-      <c r="T34" s="101"/>
-      <c r="U34" s="101"/>
-      <c r="V34" s="101"/>
-      <c r="W34" s="102"/>
-      <c r="X34" s="103"/>
-      <c r="Y34" s="34"/>
-      <c r="Z34" s="34"/>
-      <c r="AA34" s="34"/>
-      <c r="AB34" s="137"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="99"/>
+      <c r="T34" s="99"/>
+      <c r="U34" s="99"/>
+      <c r="V34" s="99"/>
+      <c r="W34" s="100"/>
+      <c r="X34" s="101"/>
+      <c r="Y34" s="33"/>
+      <c r="Z34" s="33"/>
+      <c r="AA34" s="33"/>
+      <c r="AB34" s="136"/>
     </row>
     <row r="35" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A35" s="50">
+      <c r="A35" s="49">
         <v>11</v>
       </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="73"/>
-      <c r="S35" s="101"/>
-      <c r="T35" s="101"/>
-      <c r="U35" s="101"/>
-      <c r="V35" s="101"/>
-      <c r="W35" s="102"/>
-      <c r="X35" s="103"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="34"/>
-      <c r="AA35" s="34"/>
-      <c r="AB35" s="137"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="72"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="99"/>
+      <c r="T35" s="99"/>
+      <c r="U35" s="99"/>
+      <c r="V35" s="99"/>
+      <c r="W35" s="100"/>
+      <c r="X35" s="101"/>
+      <c r="Y35" s="33"/>
+      <c r="Z35" s="33"/>
+      <c r="AA35" s="33"/>
+      <c r="AB35" s="136"/>
     </row>
     <row r="36" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A36" s="50">
+      <c r="A36" s="49">
         <v>12</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="101"/>
-      <c r="T36" s="101"/>
-      <c r="U36" s="101"/>
-      <c r="V36" s="101"/>
-      <c r="W36" s="102"/>
-      <c r="X36" s="103"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
-      <c r="AB36" s="137"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="72"/>
+      <c r="O36" s="72"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="99"/>
+      <c r="T36" s="99"/>
+      <c r="U36" s="99"/>
+      <c r="V36" s="99"/>
+      <c r="W36" s="100"/>
+      <c r="X36" s="101"/>
+      <c r="Y36" s="33"/>
+      <c r="Z36" s="33"/>
+      <c r="AA36" s="33"/>
+      <c r="AB36" s="136"/>
     </row>
     <row r="37" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A37" s="50">
+      <c r="A37" s="49">
         <v>13</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="73"/>
-      <c r="M37" s="73"/>
-      <c r="N37" s="73"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="73"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="101"/>
-      <c r="T37" s="101"/>
-      <c r="U37" s="101"/>
-      <c r="V37" s="101"/>
-      <c r="W37" s="102"/>
-      <c r="X37" s="103"/>
-      <c r="Y37" s="34"/>
-      <c r="Z37" s="34"/>
-      <c r="AA37" s="34"/>
-      <c r="AB37" s="137"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="72"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="72"/>
+      <c r="R37" s="72"/>
+      <c r="S37" s="99"/>
+      <c r="T37" s="99"/>
+      <c r="U37" s="99"/>
+      <c r="V37" s="99"/>
+      <c r="W37" s="100"/>
+      <c r="X37" s="101"/>
+      <c r="Y37" s="33"/>
+      <c r="Z37" s="33"/>
+      <c r="AA37" s="33"/>
+      <c r="AB37" s="136"/>
     </row>
     <row r="38" ht="21.65" customHeight="1" spans="1:28">
-      <c r="A38" s="52">
+      <c r="A38" s="51">
         <v>14</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="104"/>
-      <c r="T38" s="104"/>
-      <c r="U38" s="104"/>
-      <c r="V38" s="104"/>
-      <c r="W38" s="105"/>
-      <c r="X38" s="106"/>
-      <c r="Y38" s="44"/>
-      <c r="Z38" s="44"/>
-      <c r="AA38" s="44"/>
-      <c r="AB38" s="138"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="73"/>
+      <c r="S38" s="102"/>
+      <c r="T38" s="102"/>
+      <c r="U38" s="102"/>
+      <c r="V38" s="102"/>
+      <c r="W38" s="103"/>
+      <c r="X38" s="104"/>
+      <c r="Y38" s="43"/>
+      <c r="Z38" s="43"/>
+      <c r="AA38" s="43"/>
+      <c r="AB38" s="137"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="25.15" customHeight="1" spans="1:28">
-      <c r="A39" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="46"/>
-      <c r="S39" s="46"/>
-      <c r="T39" s="46"/>
-      <c r="U39" s="46" t="s">
+      <c r="A39" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="V39" s="46"/>
-      <c r="W39" s="46"/>
-      <c r="X39" s="46"/>
-      <c r="Y39" s="46"/>
-      <c r="Z39" s="46" t="s">
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="AA39" s="46"/>
-      <c r="AB39" s="135"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="45"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="134"/>
     </row>
     <row r="40" ht="25.15" customHeight="1" spans="1:28">
-      <c r="A40" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="75" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q40" s="107"/>
-      <c r="R40" s="107"/>
-      <c r="S40" s="107"/>
-      <c r="T40" s="108"/>
-      <c r="U40" s="75" t="s">
+      <c r="A40" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="V40" s="107"/>
-      <c r="W40" s="107"/>
-      <c r="X40" s="107"/>
-      <c r="Y40" s="108"/>
-      <c r="Z40" s="59"/>
-      <c r="AA40" s="59"/>
-      <c r="AB40" s="139"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q40" s="105"/>
+      <c r="R40" s="105"/>
+      <c r="S40" s="105"/>
+      <c r="T40" s="106"/>
+      <c r="U40" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="V40" s="105"/>
+      <c r="W40" s="105"/>
+      <c r="X40" s="105"/>
+      <c r="Y40" s="106"/>
+      <c r="Z40" s="58"/>
+      <c r="AA40" s="58"/>
+      <c r="AB40" s="138"/>
     </row>
     <row r="41" ht="25.15" customHeight="1" spans="1:28">
-      <c r="A41" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="60"/>
-      <c r="L41" s="60"/>
-      <c r="M41" s="60"/>
-      <c r="N41" s="60"/>
-      <c r="O41" s="60"/>
-      <c r="P41" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q41" s="60"/>
-      <c r="R41" s="60"/>
-      <c r="S41" s="60"/>
-      <c r="T41" s="60"/>
-      <c r="U41" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="V41" s="59"/>
-      <c r="W41" s="59"/>
-      <c r="X41" s="59"/>
-      <c r="Y41" s="59"/>
-      <c r="Z41" s="59"/>
-      <c r="AA41" s="59"/>
-      <c r="AB41" s="139"/>
+      <c r="A41" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+      <c r="O41" s="59"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="59"/>
+      <c r="R41" s="59"/>
+      <c r="S41" s="59"/>
+      <c r="T41" s="59"/>
+      <c r="U41" s="58"/>
+      <c r="V41" s="58"/>
+      <c r="W41" s="58"/>
+      <c r="X41" s="58"/>
+      <c r="Y41" s="58"/>
+      <c r="Z41" s="58"/>
+      <c r="AA41" s="58"/>
+      <c r="AB41" s="138"/>
     </row>
     <row r="42" ht="25.15" customHeight="1" spans="1:28">
-      <c r="A42" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="61">
-        <v>43754</v>
-      </c>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="60"/>
-      <c r="M42" s="60"/>
-      <c r="N42" s="60"/>
-      <c r="O42" s="60"/>
-      <c r="P42" s="61">
-        <v>43754</v>
-      </c>
-      <c r="Q42" s="60"/>
-      <c r="R42" s="60"/>
-      <c r="S42" s="60"/>
-      <c r="T42" s="60"/>
-      <c r="U42" s="109">
-        <v>43754</v>
-      </c>
-      <c r="V42" s="59"/>
-      <c r="W42" s="59"/>
-      <c r="X42" s="59"/>
-      <c r="Y42" s="59"/>
-      <c r="Z42" s="59"/>
-      <c r="AA42" s="59"/>
-      <c r="AB42" s="139"/>
+      <c r="A42" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="107"/>
+      <c r="V42" s="58"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="58"/>
+      <c r="Y42" s="58"/>
+      <c r="Z42" s="58"/>
+      <c r="AA42" s="58"/>
+      <c r="AB42" s="138"/>
     </row>
     <row r="43" ht="57.65" customHeight="1" spans="1:28">
-      <c r="A43" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="64"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="64"/>
-      <c r="M43" s="64"/>
-      <c r="N43" s="64"/>
-      <c r="O43" s="64"/>
-      <c r="P43" s="64"/>
-      <c r="Q43" s="64"/>
-      <c r="R43" s="64"/>
-      <c r="S43" s="64"/>
-      <c r="T43" s="64"/>
-      <c r="U43" s="64"/>
-      <c r="V43" s="64"/>
-      <c r="W43" s="64"/>
-      <c r="X43" s="64"/>
-      <c r="Y43" s="64"/>
-      <c r="Z43" s="64"/>
-      <c r="AA43" s="64"/>
-      <c r="AB43" s="140"/>
+      <c r="A43" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="63"/>
+      <c r="S43" s="63"/>
+      <c r="T43" s="63"/>
+      <c r="U43" s="63"/>
+      <c r="V43" s="63"/>
+      <c r="W43" s="63"/>
+      <c r="X43" s="63"/>
+      <c r="Y43" s="63"/>
+      <c r="Z43" s="63"/>
+      <c r="AA43" s="63"/>
+      <c r="AB43" s="139"/>
     </row>
     <row r="44" ht="16.15" customHeight="1" spans="1:28">
-      <c r="A44" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
-      <c r="L44" s="66"/>
-      <c r="M44" s="66"/>
-      <c r="N44" s="66"/>
-      <c r="O44" s="66"/>
-      <c r="P44" s="66"/>
-      <c r="Q44" s="66"/>
-      <c r="R44" s="66"/>
-      <c r="S44" s="66"/>
-      <c r="T44" s="66"/>
-      <c r="U44" s="66"/>
-      <c r="V44" s="66"/>
-      <c r="W44" s="66"/>
-      <c r="X44" s="66"/>
-      <c r="Y44" s="66"/>
-      <c r="Z44" s="66"/>
-      <c r="AA44" s="66"/>
-      <c r="AB44" s="66"/>
+      <c r="A44" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="65"/>
+      <c r="M44" s="65"/>
+      <c r="N44" s="65"/>
+      <c r="O44" s="65"/>
+      <c r="P44" s="65"/>
+      <c r="Q44" s="65"/>
+      <c r="R44" s="65"/>
+      <c r="S44" s="65"/>
+      <c r="T44" s="65"/>
+      <c r="U44" s="65"/>
+      <c r="V44" s="65"/>
+      <c r="W44" s="65"/>
+      <c r="X44" s="65"/>
+      <c r="Y44" s="65"/>
+      <c r="Z44" s="65"/>
+      <c r="AA44" s="65"/>
+      <c r="AB44" s="65"/>
     </row>
     <row r="45" ht="21.65" customHeight="1"/>
     <row r="46" ht="21.65" customHeight="1" spans="11:11">
-      <c r="K46" s="76"/>
+      <c r="K46" s="74"/>
     </row>
     <row r="47" ht="21.65" customHeight="1"/>
     <row r="48" ht="21.65" customHeight="1"/>
@@ -7031,10 +6990,10 @@
   <headerFooter/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="11268" name="Check Box 4" r:id="rId4">
               <controlPr defaultSize="0">
@@ -7056,7 +7015,7 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="11269" name="Check Box 5" r:id="rId5">
               <controlPr defaultSize="0">

</xml_diff>

<commit_message>
Ekipman bilgilerinde cihaz adını seçtiğimde diğer bilgileri çağırabildim,ilk ekrandan seçtiğim personel bilgilerini rapordaki personel tablosuna akardım ve en son bu bilgileri excele aktardım.
</commit_message>
<xml_diff>
--- a/newProjekt/MagneticReport.xlsx
+++ b/newProjekt/MagneticReport.xlsx
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -2618,6 +2618,36 @@
   </si>
   <si>
     <t>Doküman No: F.02 Yayın Tarihi : 01.05.2018 Revizyon No :01 Revizyon Tarihi :19.03.2019</t>
+  </si>
+  <si>
+    <t>ARSLAN GEMİ</t>
+  </si>
+  <si>
+    <t>şeyma yılmaz</t>
+  </si>
+  <si>
+    <t>berra kalem</t>
+  </si>
+  <si>
+    <t>seviye 1</t>
+  </si>
+  <si>
+    <t>100 mm</t>
+  </si>
+  <si>
+    <t>NAWOO Sn:1701020</t>
+  </si>
+  <si>
+    <t>sena oglak</t>
+  </si>
+  <si>
+    <t>150mm</t>
+  </si>
+  <si>
+    <t>NAWOO Sn:1801040</t>
+  </si>
+  <si>
+    <t>Seviye 3</t>
   </si>
 </sst>
 </file>
@@ -3808,7 +3838,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4222,6 +4252,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -4787,32 +4835,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81904761904762" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.26666666666667" style="3" customWidth="1"/>
-    <col min="2" max="3" width="5.26666666666667" style="3" customWidth="1"/>
-    <col min="4" max="4" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4.72380952380952" style="3" customWidth="1"/>
-    <col min="6" max="6" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="7" max="7" width="4.18095238095238" style="3" customWidth="1"/>
-    <col min="8" max="8" width="3.26666666666667" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.54285714285714" style="3" customWidth="1"/>
-    <col min="10" max="10" width="3.45714285714286" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.72380952380952" style="3" customWidth="1"/>
-    <col min="12" max="12" width="4.81904761904762" style="3" customWidth="1"/>
-    <col min="13" max="15" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.72380952380952" style="3" customWidth="1"/>
-    <col min="17" max="17" width="3.72380952380952" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.7238095238095" style="3" customWidth="1"/>
-    <col min="19" max="19" width="4.81904761904762" style="3" customWidth="1"/>
-    <col min="20" max="20" width="3.81904761904762" style="3" customWidth="1"/>
-    <col min="21" max="21" width="3.45714285714286" style="3" customWidth="1"/>
-    <col min="22" max="22" width="0.819047619047619" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.7238095238095" style="3" customWidth="1"/>
-    <col min="24" max="24" width="2.45714285714286" style="3" customWidth="1"/>
-    <col min="25" max="25" width="5.72380952380952" style="3" customWidth="1"/>
-    <col min="26" max="26" width="4.72380952380952" style="3" customWidth="1"/>
-    <col min="27" max="27" width="6.72380952380952" style="3" customWidth="1"/>
-    <col min="28" max="28" width="7.81904761904762" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="8.81904761904762" style="3"/>
+    <col min="1" max="1" customWidth="true" style="3" width="7.26666666666667" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="3" width="5.26666666666667" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="4.18095238095238" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="3.26666666666667" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="5.54285714285714" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
+    <col min="13" max="15" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="3" width="8.72380952380952" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="3" width="3.72380952380952" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="3" width="4.81904761904762" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="3" width="3.81904761904762" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="3" width="3.45714285714286" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="3" width="0.819047619047619" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="3" width="10.7238095238095" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="3" width="2.45714285714286" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="3" width="5.72380952380952" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="3" width="4.72380952380952" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="3" width="6.72380952380952" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="3" width="7.81904761904762" collapsed="true"/>
+    <col min="29" max="16384" style="3" width="8.81904761904762" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="31.9" customHeight="1" spans="1:28">
@@ -4885,8 +4933,8 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="14" t="s">
-        <v>3</v>
+      <c r="D3" t="s" s="145">
+        <v>83</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -4923,7 +4971,7 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="14" t="s">
+      <c r="D4" t="s" s="145">
         <v>7</v>
       </c>
       <c r="E4" s="18"/>
@@ -4961,7 +5009,7 @@
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
-      <c r="D5" s="14" t="s">
+      <c r="D5" t="s" s="145">
         <v>11</v>
       </c>
       <c r="E5" s="18"/>
@@ -5103,8 +5151,12 @@
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="D9" t="s" s="143">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s" s="145">
+        <v>90</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -5139,8 +5191,12 @@
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="D10" t="s" s="143">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s" s="145">
+        <v>91</v>
+      </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -6235,7 +6291,7 @@
       <c r="C40" s="57"/>
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
-      <c r="F40" s="14" t="s">
+      <c r="F40" t="s" s="145">
         <v>76</v>
       </c>
       <c r="G40" s="58"/>
@@ -6247,15 +6303,15 @@
       <c r="M40" s="58"/>
       <c r="N40" s="58"/>
       <c r="O40" s="58"/>
-      <c r="P40" s="14" t="s">
+      <c r="P40" t="s" s="145">
         <v>77</v>
       </c>
       <c r="Q40" s="105"/>
       <c r="R40" s="105"/>
       <c r="S40" s="105"/>
       <c r="T40" s="106"/>
-      <c r="U40" s="14" t="s">
-        <v>78</v>
+      <c r="U40" t="s" s="145">
+        <v>84</v>
       </c>
       <c r="V40" s="105"/>
       <c r="W40" s="105"/>
@@ -6273,7 +6329,9 @@
       <c r="C41" s="57"/>
       <c r="D41" s="57"/>
       <c r="E41" s="57"/>
-      <c r="F41" s="59"/>
+      <c r="F41" t="s" s="145">
+        <v>86</v>
+      </c>
       <c r="G41" s="59"/>
       <c r="H41" s="59"/>
       <c r="I41" s="59"/>
@@ -6283,12 +6341,16 @@
       <c r="M41" s="59"/>
       <c r="N41" s="59"/>
       <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
+      <c r="P41" t="s" s="145">
+        <v>92</v>
+      </c>
       <c r="Q41" s="59"/>
       <c r="R41" s="59"/>
       <c r="S41" s="59"/>
       <c r="T41" s="59"/>
-      <c r="U41" s="58"/>
+      <c r="U41" t="s" s="145">
+        <v>92</v>
+      </c>
       <c r="V41" s="58"/>
       <c r="W41" s="58"/>
       <c r="X41" s="58"/>
@@ -6990,10 +7052,10 @@
   <headerFooter/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x14">
       <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:AlternateContent>
           <mc:Choice Requires="x14">
             <control shapeId="11268" name="Check Box 4" r:id="rId4">
               <controlPr defaultSize="0">
@@ -7015,7 +7077,7 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:AlternateContent>
           <mc:Choice Requires="x14">
             <control shapeId="11269" name="Check Box 5" r:id="rId5">
               <controlPr defaultSize="0">

</xml_diff>

<commit_message>
OOP mantığına uygun olarak düzenledim.
</commit_message>
<xml_diff>
--- a/newProjekt/MagneticReport.xlsx
+++ b/newProjekt/MagneticReport.xlsx
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="95">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -2651,6 +2651,9 @@
   </si>
   <si>
     <t>seviye 2</t>
+  </si>
+  <si>
+    <t>Seviye 2</t>
   </si>
 </sst>
 </file>
@@ -3841,7 +3844,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4255,6 +4258,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4960,7 +4969,7 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" t="s" s="153">
+      <c r="D3" t="s" s="155">
         <v>3</v>
       </c>
       <c r="E3" s="15"/>
@@ -4998,7 +5007,7 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
-      <c r="D4" t="s" s="153">
+      <c r="D4" t="s" s="155">
         <v>7</v>
       </c>
       <c r="E4" s="18"/>
@@ -5036,7 +5045,7 @@
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
-      <c r="D5" t="s" s="153">
+      <c r="D5" t="s" s="155">
         <v>11</v>
       </c>
       <c r="E5" s="18"/>
@@ -5181,8 +5190,8 @@
       <c r="D9" t="s" s="143">
         <v>87</v>
       </c>
-      <c r="E9" t="s" s="153">
-        <v>90</v>
+      <c r="E9" t="s" s="155">
+        <v>87</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -5221,8 +5230,8 @@
       <c r="D10" t="s" s="143">
         <v>88</v>
       </c>
-      <c r="E10" t="s" s="153">
-        <v>91</v>
+      <c r="E10" t="s" s="155">
+        <v>88</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -6318,7 +6327,7 @@
       <c r="C40" s="57"/>
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
-      <c r="F40" t="s" s="153">
+      <c r="F40" t="s" s="155">
         <v>76</v>
       </c>
       <c r="G40" s="58"/>
@@ -6330,14 +6339,14 @@
       <c r="M40" s="58"/>
       <c r="N40" s="58"/>
       <c r="O40" s="58"/>
-      <c r="P40" t="s" s="153">
+      <c r="P40" t="s" s="155">
         <v>77</v>
       </c>
       <c r="Q40" s="105"/>
       <c r="R40" s="105"/>
       <c r="S40" s="105"/>
       <c r="T40" s="106"/>
-      <c r="U40" t="s" s="153">
+      <c r="U40" t="s" s="155">
         <v>78</v>
       </c>
       <c r="V40" s="105"/>
@@ -6356,7 +6365,7 @@
       <c r="C41" s="57"/>
       <c r="D41" s="57"/>
       <c r="E41" s="57"/>
-      <c r="F41" t="s" s="153">
+      <c r="F41" t="s" s="155">
         <v>86</v>
       </c>
       <c r="G41" s="59"/>
@@ -6368,15 +6377,15 @@
       <c r="M41" s="59"/>
       <c r="N41" s="59"/>
       <c r="O41" s="59"/>
-      <c r="P41" t="s" s="153">
+      <c r="P41" t="s" s="155">
         <v>92</v>
       </c>
       <c r="Q41" s="59"/>
       <c r="R41" s="59"/>
       <c r="S41" s="59"/>
       <c r="T41" s="59"/>
-      <c r="U41" t="s" s="153">
-        <v>92</v>
+      <c r="U41" t="s" s="155">
+        <v>94</v>
       </c>
       <c r="V41" s="58"/>
       <c r="W41" s="58"/>

</xml_diff>